<commit_message>
Plantilla e importación de horas extras
Plantilla e importación de horas extras
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_horas_extra.xlsx
+++ b/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_horas_extra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INCOE\Documents\GitHub\fe\location\l10n_sv_hr_asignaciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D971DD2D-6B79-466B-A883-D7958A61387B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09828EBC-7BAD-40F0-8C5D-2A887555E6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1065" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Horas Extra" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Empleado</t>
   </si>
@@ -110,10 +110,7 @@
     <t>Horas nocturnas en día de asueto</t>
   </si>
   <si>
-    <t>Periodo</t>
-  </si>
-  <si>
-    <t>Código de Empleado</t>
+    <t>codigo_empleado</t>
   </si>
 </sst>
 </file>
@@ -145,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -153,30 +150,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,32 +483,35 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Modificación en plantilla de horas extras
Modificación en plantilla de horas extras
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_horas_extra.xlsx
+++ b/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_horas_extra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INCOE\Documents\GitHub\fe\location\l10n_sv_hr_asignaciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EC89C5-127C-4BAD-8C0A-FE05111AC851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265895B8-F725-40DF-88B2-B5D0C9C21CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1065" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,24 @@
     <sheet name="Horas Extra" sheetId="1" r:id="rId1"/>
     <sheet name="Guía" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Empleado</t>
   </si>
@@ -111,6 +123,18 @@
   </si>
   <si>
     <t>codigo_empleado</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>Tipo de horas</t>
+  </si>
+  <si>
+    <t>Horas extras</t>
+  </si>
+  <si>
+    <t>Viáticos</t>
   </si>
 </sst>
 </file>
@@ -463,75 +487,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BF95382-D2FD-4F42-BEB8-9F8271D8D395}">
+          <x14:formula1>
+            <xm:f>Guía!$B$11:$B$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -643,6 +691,19 @@
         <v>28</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Modificacion en plantilla de asignaciones
Modificacion en plantilla de asignaciones
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_horas_extra.xlsx
+++ b/location/l10n_sv_hr_asignaciones/static/src/plantilla/plantilla_horas_extra.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INCOE\Documents\GitHub\fe\location\l10n_sv_hr_asignaciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265895B8-F725-40DF-88B2-B5D0C9C21CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF07B04E-45F4-44C8-B993-C36368665D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1065" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28905" yWindow="1185" windowWidth="29010" windowHeight="7845" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Horas Extra" sheetId="1" r:id="rId1"/>
-    <sheet name="Guía" sheetId="2" r:id="rId2"/>
+    <sheet name="Guía" sheetId="2" r:id="rId1"/>
+    <sheet name="Horas Extra" sheetId="1" r:id="rId2"/>
+    <sheet name="Asignaciones" sheetId="4" r:id="rId3"/>
+    <sheet name="OpcionesTipo" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>Empleado</t>
   </si>
@@ -128,13 +130,46 @@
     <t>tipo</t>
   </si>
   <si>
-    <t>Tipo de horas</t>
-  </si>
-  <si>
-    <t>Horas extras</t>
-  </si>
-  <si>
-    <t>Viáticos</t>
+    <t>HORAS EXTRAS</t>
+  </si>
+  <si>
+    <t>COMISION</t>
+  </si>
+  <si>
+    <t>VIATICO</t>
+  </si>
+  <si>
+    <t>BONO</t>
+  </si>
+  <si>
+    <t>monto</t>
+  </si>
+  <si>
+    <t>Bienvenido al archivo de importación de asignaciones salariales.</t>
+  </si>
+  <si>
+    <t>El archivo contiene tres pestañas:</t>
+  </si>
+  <si>
+    <t>- 'Horas Extras': solo para registrar horas extras.</t>
+  </si>
+  <si>
+    <t>- 'Asignaciones': para otros tipos como COMISION, VIATICO o BONO.</t>
+  </si>
+  <si>
+    <t>- 'OpcionesTipo': hoja técnica con los valores válidos para el campo 'tipo'. No modificar.</t>
+  </si>
+  <si>
+    <t>⚠ Importante:</t>
+  </si>
+  <si>
+    <t>- No borrar ni cambiar los nombres de las hojas.</t>
+  </si>
+  <si>
+    <t>- El campo 'tipo' es obligatorio.</t>
+  </si>
+  <si>
+    <t>- En 'Horas Extras', se deben completar al menos una de las columnas de horas.</t>
   </si>
 </sst>
 </file>
@@ -486,25 +521,201 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -552,12 +763,18 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BF95382-D2FD-4F42-BEB8-9F8271D8D395}">
           <x14:formula1>
             <xm:f>Guía!$B$11:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
+          <xm:sqref>B1 B3:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6950ADE9-E2C2-4377-991B-FBFC812F2495}">
+          <x14:formula1>
+            <xm:f>OpcionesTipo!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -565,146 +782,109 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C12"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB4BDFD-FBAC-4B96-836E-5AF86AA041A1}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BE7FE6C6-2B0D-4C6B-855D-B18CBC410611}">
+          <x14:formula1>
+            <xm:f>Guía!$B$11:$B$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9BFC39DE-0A78-46B1-B0BE-EC5C226DD98F}">
+          <x14:formula1>
+            <xm:f>OpcionesTipo!$A$3:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843A48C3-0FDE-4B0D-BEA2-0E06BC56A8E7}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kpnTmtWGxoWSJz8BSuNTj4GgSVAXOkcWPjlpyYjRF+UUFcJbDpcHmGb6Fk4ovk8fkNqX17QEFzUu237TDh8t9Q==" saltValue="LIBin5KXRuqB3fjPpTUK1g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>